<commit_message>
creacion de destruir.php y cambio de redireccionamiento en salas.php
</commit_message>
<xml_diff>
--- a/Gestión/Plantilla Scrum daily meeting.xlsx
+++ b/Gestión/Plantilla Scrum daily meeting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\DAW2\M12\PROYECYO RESTAURANTE\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AE47F8-938F-41A0-B41F-0DA8B0A3D7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBD80E1-30BB-483E-8F48-20972460EDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,15 +337,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -961,19 +952,19 @@
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="3">
         <v>45603</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="17" t="s">
@@ -1004,19 +995,19 @@
       <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="3">
         <v>45603</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="17" t="s">

</xml_diff>